<commit_message>
PLSstatic geeft output, twijfel of het klopt
</commit_message>
<xml_diff>
--- a/results_PLSstatic_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
+++ b/results_PLSstatic_with_AIC_BIC_AdjustedR2_LogLikelihood_Residuals.xlsx
@@ -456,17 +456,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>RMSE_OutSample</t>
+          <t>RMSE_TestSample</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>R2_OutSample</t>
+          <t>R2_TestSample</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Adjusted_R2_OutSample</t>
+          <t>Adjusted_R2_TestSample</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -499,13 +499,13 @@
         <v>0.7747294475835051</v>
       </c>
       <c r="E2" t="n">
-        <v>1.108808755024328</v>
+        <v>0.2203059453264854</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.6551338194126273</v>
+        <v>0.8110024965460946</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.8569794071458743</v>
+        <v>0.79350272770777</v>
       </c>
       <c r="H2" t="n">
         <v>-148.9208377394731</v>
@@ -531,13 +531,13 @@
         <v>0.8010436971167462</v>
       </c>
       <c r="E3" t="n">
-        <v>1.116364678265628</v>
+        <v>0.2227255026184086</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.7165082877823423</v>
+        <v>0.7884419990383102</v>
       </c>
       <c r="G3" t="n">
-        <v>-0.9739845309496935</v>
+        <v>0.7644920366652888</v>
       </c>
       <c r="H3" t="n">
         <v>-140.0084339213685</v>
@@ -563,13 +563,13 @@
         <v>0.8191240061448376</v>
       </c>
       <c r="E4" t="n">
-        <v>1.113607681171743</v>
+        <v>0.219499513946479</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.7064148397641534</v>
+        <v>0.8018701931147736</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.012694426388489</v>
+        <v>0.775198872957147</v>
       </c>
       <c r="H4" t="n">
         <v>-119.4674943522318</v>
@@ -595,13 +595,13 @@
         <v>0.8407007150837069</v>
       </c>
       <c r="E5" t="n">
-        <v>1.113114082651026</v>
+        <v>0.2056537017474372</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.7062427681643426</v>
+        <v>0.8528421542171547</v>
       </c>
       <c r="G5" t="n">
-        <v>-1.065451771988415</v>
+        <v>0.8297585705649437</v>
       </c>
       <c r="H5" t="n">
         <v>-88.41607213641095</v>
@@ -627,13 +627,13 @@
         <v>0.8562910372067848</v>
       </c>
       <c r="E6" t="n">
-        <v>1.118098755793166</v>
+        <v>0.207149563537544</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.7396940492656203</v>
+        <v>0.8415319424109894</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.16286287205996</v>
+        <v>0.8130076920449675</v>
       </c>
       <c r="H6" t="n">
         <v>-76.46575018245896</v>
@@ -659,13 +659,13 @@
         <v>0.8678806665659624</v>
       </c>
       <c r="E7" t="n">
-        <v>1.116717017704071</v>
+        <v>0.2047829187007655</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.7314071915007834</v>
+        <v>0.8430252898723016</v>
       </c>
       <c r="G7" t="n">
-        <v>-1.212353633584334</v>
+        <v>0.8109896347441999</v>
       </c>
       <c r="H7" t="n">
         <v>-74.52490467644175</v>
@@ -691,13 +691,13 @@
         <v>0.8775863368290787</v>
       </c>
       <c r="E8" t="n">
-        <v>1.110043759904843</v>
+        <v>0.1908189957460074</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.6764347707374372</v>
+        <v>0.8732255329845089</v>
       </c>
       <c r="G8" t="n">
-        <v>-1.20331427011206</v>
+        <v>0.8441730509601255</v>
       </c>
       <c r="H8" t="n">
         <v>-56.92215246145511</v>
@@ -723,13 +723,13 @@
         <v>0.8886497648374425</v>
       </c>
       <c r="E9" t="n">
-        <v>1.109418810498657</v>
+        <v>0.1891215040397849</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.6674325561341061</v>
+        <v>0.8780378382793181</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.255938164181438</v>
+        <v>0.8468985629463781</v>
       </c>
       <c r="H9" t="n">
         <v>-49.0989284564281</v>

</xml_diff>